<commit_message>
risoluzione problema inserimento dati post aggiornamento DB
</commit_message>
<xml_diff>
--- a/dati_soci.xlsx
+++ b/dati_soci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -40,16 +40,16 @@
     <t>inviato</t>
   </si>
   <si>
-    <t xml:space="preserve"> w</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>w@ww.it</t>
-  </si>
-  <si>
-    <t>Screenshot 2024-10-20 alle 22.11.34.png</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>a@a.it</t>
+  </si>
+  <si>
+    <t>Screenshot 2024-08-30 alle 15.56.50.png</t>
+  </si>
+  <si>
+    <t>Screenshot 2024-10-21 alle 20.27.06.png</t>
   </si>
   <si>
     <t>SI</t>
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,27 +444,44 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>1201</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
risoluzione problema inserimento dati post update DB
</commit_message>
<xml_diff>
--- a/dati_soci.xlsx
+++ b/dati_soci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>a@a.it</t>
-  </si>
-  <si>
-    <t>Screenshot 2024-08-30 alle 15.56.50.png</t>
   </si>
   <si>
     <t>Screenshot 2024-10-21 alle 20.27.06.png</t>
@@ -410,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,7 +441,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -458,31 +455,14 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3">
+      <c r="G2">
         <v>1201</v>
       </c>
-      <c r="H3" t="s">
-        <v>12</v>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
risoluzione aggiornamento dati post UPDATE DB
</commit_message>
<xml_diff>
--- a/dati_soci.xlsx
+++ b/dati_soci.xlsx
@@ -40,10 +40,10 @@
     <t>inviato</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>a@a.it</t>
+    <t>b</t>
+  </si>
+  <si>
+    <t>b@b.it</t>
   </si>
   <si>
     <t>Screenshot 2024-10-21 alle 20.27.06.png</t>

</xml_diff>

<commit_message>
risoluzione problema aggiornamento DB e nuovi dati html
</commit_message>
<xml_diff>
--- a/dati_soci.xlsx
+++ b/dati_soci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -40,22 +40,85 @@
     <t>inviato</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>a@a.it</t>
-  </si>
-  <si>
-    <t>s@s.it</t>
-  </si>
-  <si>
-    <t>Screenshot 2024-10-21 alle 20.27.06.png</t>
-  </si>
-  <si>
-    <t>domenica_eliminatorie.png</t>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Giulia</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Francesco</t>
+  </si>
+  <si>
+    <t>giuseppe</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Rossi</t>
+  </si>
+  <si>
+    <t>Bianchi</t>
+  </si>
+  <si>
+    <t>Neri</t>
+  </si>
+  <si>
+    <t>Gallo</t>
+  </si>
+  <si>
+    <t>cangemi</t>
+  </si>
+  <si>
+    <t>Verdi</t>
+  </si>
+  <si>
+    <t>luca.rossi@example.com</t>
+  </si>
+  <si>
+    <t>giulia.bianchi@example.com</t>
+  </si>
+  <si>
+    <t>sara.neri@example.com</t>
+  </si>
+  <si>
+    <t>francesco.gallo@example.com</t>
+  </si>
+  <si>
+    <t>giuseppecangemi94@gmail.com</t>
+  </si>
+  <si>
+    <t>aaa@aaa.it</t>
+  </si>
+  <si>
+    <t>marco.verdi@example.com</t>
+  </si>
+  <si>
+    <t>file1.pdf</t>
+  </si>
+  <si>
+    <t>file2.pdf</t>
+  </si>
+  <si>
+    <t>file4.pdf</t>
+  </si>
+  <si>
+    <t>file5.pdf</t>
+  </si>
+  <si>
+    <t>Schermata 2021-09-24 alle 13.37.38.png</t>
+  </si>
+  <si>
+    <t>Schermata 2019-06-13 alle 19.28.40.png</t>
+  </si>
+  <si>
+    <t>file3.pdf</t>
   </si>
   <si>
     <t>SI</t>
@@ -416,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,13 +519,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -473,22 +536,116 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6">
+        <v>1201</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="G3">
-        <v>1201</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>1202</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
numero tessera da poter scegliere
</commit_message>
<xml_diff>
--- a/dati_soci.xlsx
+++ b/dati_soci.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1087,6 +1087,128 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
     </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Giuseppe</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Cangemi</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>giuseppecangemi94@gmail.com</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>derryrockfoto.jpg</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pinco </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Pallino</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>savvoz@pinko.com</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1000052151.jpg</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Luca </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Era Gay</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>LucaKastlewave@gmail.com</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1000052725.jpg</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Giuseppe</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Cangemi</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>giuseppecangemi94@gmail.com</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>derryrockfoto.jpg</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>1209</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>